<commit_message>
gatos del 08/10/2022 y el 13/10/2022
</commit_message>
<xml_diff>
--- a/Gastos.xlsx
+++ b/Gastos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Datos Dico D Backup\Gastos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D546C4AF-CBD8-4A17-8AA0-107DA8D0CFBE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F051E5-C4F2-45A5-8B3F-EEC9DF06C1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{04CEE15F-19F2-4642-940D-458436DFBC61}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Inversion marranos cantidad 2</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>cascarilla de arroz</t>
+  </si>
+  <si>
+    <t>construccion chiquero y clavos</t>
+  </si>
+  <si>
+    <t>yodo y guantes</t>
   </si>
 </sst>
 </file>
@@ -191,8 +197,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C25EB676-D0E0-4135-B57A-56D1288FFA53}" name="Tabla1" displayName="Tabla1" ref="A1:C34" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:C34" xr:uid="{C25EB676-D0E0-4135-B57A-56D1288FFA53}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C25EB676-D0E0-4135-B57A-56D1288FFA53}" name="Tabla1" displayName="Tabla1" ref="A1:C36" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:C36" xr:uid="{C25EB676-D0E0-4135-B57A-56D1288FFA53}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{272B14D6-45DB-40F1-89C7-7BE2429F6C2E}" name="Gasto en pesos"/>
     <tableColumn id="2" xr3:uid="{7C8066EB-3B59-4EE8-9300-3B8FDFBAD3E6}" name="Detalle del gasto "/>
@@ -499,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09624448-6883-4ED2-B412-662A8D01BCFE}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -692,8 +698,8 @@
         <v>10</v>
       </c>
       <c r="G16" s="3">
-        <f>SUM(A2:A34)</f>
-        <v>2776000</v>
+        <f>SUM(A2:A36)</f>
+        <v>2829000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,6 +898,28 @@
       </c>
       <c r="C34" s="2">
         <v>44834</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>38000</v>
+      </c>
+      <c r="B35" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="2">
+        <v>44842</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>15000</v>
+      </c>
+      <c r="B36" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="2">
+        <v>44847</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Gasto ultimos dias de Octubre
</commit_message>
<xml_diff>
--- a/Gastos.xlsx
+++ b/Gastos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Datos Dico D Backup\Gastos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1F051E5-C4F2-45A5-8B3F-EEC9DF06C1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{265405A3-7FA8-4CFB-9DB6-CC6D3966AD4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{04CEE15F-19F2-4642-940D-458436DFBC61}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Inversion marranos cantidad 2</t>
   </si>
@@ -106,6 +106,12 @@
   </si>
   <si>
     <t>yodo y guantes</t>
+  </si>
+  <si>
+    <t>Gastos de Parto</t>
+  </si>
+  <si>
+    <t>Gastos de alimento de engorde</t>
   </si>
 </sst>
 </file>
@@ -197,8 +203,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C25EB676-D0E0-4135-B57A-56D1288FFA53}" name="Tabla1" displayName="Tabla1" ref="A1:C36" totalsRowShown="0" headerRowDxfId="1">
-  <autoFilter ref="A1:C36" xr:uid="{C25EB676-D0E0-4135-B57A-56D1288FFA53}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C25EB676-D0E0-4135-B57A-56D1288FFA53}" name="Tabla1" displayName="Tabla1" ref="A1:C38" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="A1:C38" xr:uid="{C25EB676-D0E0-4135-B57A-56D1288FFA53}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{272B14D6-45DB-40F1-89C7-7BE2429F6C2E}" name="Gasto en pesos"/>
     <tableColumn id="2" xr3:uid="{7C8066EB-3B59-4EE8-9300-3B8FDFBAD3E6}" name="Detalle del gasto "/>
@@ -505,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09624448-6883-4ED2-B412-662A8D01BCFE}">
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="D38" sqref="D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -698,8 +704,8 @@
         <v>10</v>
       </c>
       <c r="G16" s="3">
-        <f>SUM(A2:A36)</f>
-        <v>2829000</v>
+        <f>SUM(A2:A38)</f>
+        <v>3081000</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -920,6 +926,28 @@
       </c>
       <c r="C36" s="2">
         <v>44847</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>150000</v>
+      </c>
+      <c r="B37" t="s">
+        <v>24</v>
+      </c>
+      <c r="C37" s="2">
+        <v>44854</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>102000</v>
+      </c>
+      <c r="B38" t="s">
+        <v>25</v>
+      </c>
+      <c r="C38" s="2">
+        <v>44862</v>
       </c>
     </row>
   </sheetData>

</xml_diff>